<commit_message>
meta group switch fixed
</commit_message>
<xml_diff>
--- a/sample_file/class_list_CS_3990_5969_20191__1____moreGroups.xlsx
+++ b/sample_file/class_list_CS_3990_5969_20191__1____moreGroups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\edusample\sample_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\edusample\sample_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05206C8F-703B-41D8-BE34-3DF25ABFC3D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4481379-85BD-449D-AA93-8002F9540CB3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>Session</t>
   </si>
@@ -42,42 +42,9 @@
     <t>Student</t>
   </si>
   <si>
-    <t>Primary POS</t>
-  </si>
-  <si>
-    <t>Primary College</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Obj</t>
-  </si>
-  <si>
-    <t>Primary Program</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Hrs</t>
-  </si>
-  <si>
-    <t>P/F</t>
-  </si>
-  <si>
-    <t>Residing</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Registration Date</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -88,33 +55,6 @@
   </si>
   <si>
     <t>Zhao, Runqi</t>
-  </si>
-  <si>
-    <t>CLAS Computer Science (BS)</t>
-  </si>
-  <si>
-    <t>CLAS</t>
-  </si>
-  <si>
-    <t>Fourth Year</t>
-  </si>
-  <si>
-    <t>BS</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Enrolled</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>602 Westgate St Apt 12&lt;br/&gt;Iowa City, IA 52246-4628</t>
-  </si>
-  <si>
-    <t>319-400-8963</t>
   </si>
   <si>
     <t>runqzhao@uiowa.edu</t>
@@ -388,7 +328,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -396,18 +336,18 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -436,14 +376,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -725,18 +662,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -756,456 +693,390 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2" t="str">
         <f>"01206051"</f>
         <v>01206051</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2">
-        <v>43600</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="D3" t="s">
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7">
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7">
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="D4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="G24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7">
+      <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="D5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="D6" s="3" t="s">
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7">
+      <c r="D26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="D7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7">
+      <c r="D27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="D8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="R8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="D9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="D10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="D11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="D12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="G27" t="s">
         <v>87</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="D13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="D14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="D15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="D16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="4:18">
-      <c r="D17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="4:18">
-      <c r="D18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="4:18">
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="4:18">
-      <c r="D20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="4:18">
-      <c r="D21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="4:18">
-      <c r="D22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="4:18">
-      <c r="D23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="4:18">
-      <c r="D24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="4:18">
-      <c r="D25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="R25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="4:18">
-      <c r="D26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="R26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="4:18">
-      <c r="D27" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="R27" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{3D807735-1547-4149-81CE-15346DEF7F39}"/>
-    <hyperlink ref="O5:O27" r:id="rId4" display="c0@uiowa.edu" xr:uid="{74347AA5-12C9-4B2A-9157-AC500BEA70A9}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{3D807735-1547-4149-81CE-15346DEF7F39}"/>
+    <hyperlink ref="E5:E27" r:id="rId4" display="c0@uiowa.edu" xr:uid="{74347AA5-12C9-4B2A-9157-AC500BEA70A9}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>

</xml_diff>